<commit_message>
Lernstand update der Themen
</commit_message>
<xml_diff>
--- a/docs/material/Lernstand.xlsx
+++ b/docs/material/Lernstand.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\André Neumann\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E95485-72F7-44F8-811C-347FF43825A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1160952D-F0DA-4A3D-9A85-71E3EFEB4515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{B7884D5C-17C3-4F72-B534-6B15B5BBA262}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7884D5C-17C3-4F72-B534-6B15B5BBA262}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>Projektmanagement (div. LF)</t>
   </si>
@@ -116,6 +116,24 @@
     <t>Lernstand</t>
   </si>
   <si>
+    <t>Netzwerktechnik (LF3)</t>
+  </si>
+  <si>
+    <t>Grundkonzepte von Netzwerken beschreiben</t>
+  </si>
+  <si>
+    <t>Clients einem Netzwerk hinzufügen</t>
+  </si>
+  <si>
+    <t>OSI-Modell nutzen</t>
+  </si>
+  <si>
+    <t>Wichtige Protokolle zuordnen</t>
+  </si>
+  <si>
+    <t>UML-Klassendiagramme erstellen</t>
+  </si>
+  <si>
     <t>Anwendungsentwicklung (LF5)</t>
   </si>
   <si>
@@ -125,7 +143,7 @@
     <t>Datenbanken abfragen</t>
   </si>
   <si>
-    <t>UML-Klassendiagramme erstellen</t>
+    <t>IT-Sicherheit (LF4)</t>
   </si>
 </sst>
 </file>
@@ -184,28 +202,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -241,34 +237,127 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -663,44 +752,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DB9513-9E88-4020-9A13-204A732F2DD8}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="47.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="2.88671875" customWidth="1"/>
+    <col min="4" max="4" width="47.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="2.88671875" customWidth="1"/>
+    <col min="7" max="7" width="47.21875" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9"/>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -708,13 +801,19 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -722,13 +821,19 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -736,184 +841,179 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="D14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="G14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="9"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="G17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A22:B22"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:B8">
-    <cfRule type="cellIs" dxfId="11" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="55" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="56" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="57" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="iconSet" priority="40">
+    <cfRule type="iconSet" priority="58">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -921,8 +1021,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
-    <cfRule type="iconSet" priority="20">
+  <conditionalFormatting sqref="E4">
+    <cfRule type="iconSet" priority="38">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -930,19 +1030,19 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:B19">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+  <conditionalFormatting sqref="E4:E11">
+    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="29" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B18">
-    <cfRule type="iconSet" priority="28">
+  <conditionalFormatting sqref="E5:E10">
+    <cfRule type="iconSet" priority="46">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -950,8 +1050,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="iconSet" priority="12">
+  <conditionalFormatting sqref="E11">
+    <cfRule type="iconSet" priority="30">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -959,8 +1059,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="iconSet" priority="16">
+  <conditionalFormatting sqref="H4">
+    <cfRule type="iconSet" priority="34">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -968,19 +1068,19 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23:B29">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="H4:H10">
+    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="24" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="25" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:B28">
-    <cfRule type="iconSet" priority="24">
+  <conditionalFormatting sqref="H5:H9">
+    <cfRule type="iconSet" priority="42">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -988,7 +1088,54 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
+  <conditionalFormatting sqref="H10">
+    <cfRule type="iconSet" priority="26">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:B18">
+    <cfRule type="cellIs" dxfId="11" priority="59" operator="equal">
+      <formula>"in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="60" operator="equal">
+      <formula>"Offen"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="61" operator="equal">
+      <formula>"Erledigt"</formula>
+    </cfRule>
+    <cfRule type="iconSet" priority="62">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16:H17">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Offen"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>"Erledigt"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="iconSet" priority="9">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
     <cfRule type="iconSet" priority="8">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -997,16 +1144,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E8">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"in Bearbeitung"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"Offen"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"Erledigt"</formula>
-    </cfRule>
+  <conditionalFormatting sqref="H15">
     <cfRule type="iconSet" priority="4">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1015,8 +1153,19 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Offen"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Erledigt"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C8 B23:B29 B12:B19 F4:F11 E4:E8" xr:uid="{EC34E9F4-7F72-4106-BC88-1EE30967E81D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C8 E4:F11 H4:H10 B15:B18 H15:H17" xr:uid="{EC34E9F4-7F72-4106-BC88-1EE30967E81D}">
       <formula1>"Offen, in Bearbeitung, Erledigt"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Tabelle für den Lernstand mit Themen aktualisiert
</commit_message>
<xml_diff>
--- a/docs/material/Lernstand.xlsx
+++ b/docs/material/Lernstand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\André Neumann\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\GitHub\MMBbS_KIT_PVAP1\docs\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1160952D-F0DA-4A3D-9A85-71E3EFEB4515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E72F58-C897-479D-9249-1A9947046433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7884D5C-17C3-4F72-B534-6B15B5BBA262}"/>
+    <workbookView xWindow="17970" yWindow="16035" windowWidth="20295" windowHeight="15525" xr2:uid="{B7884D5C-17C3-4F72-B534-6B15B5BBA262}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>Projektmanagement (div. LF)</t>
   </si>
@@ -140,10 +140,31 @@
     <t>Datenbanken mit ER-Modellen planen</t>
   </si>
   <si>
-    <t>Datenbanken abfragen</t>
-  </si>
-  <si>
     <t>IT-Sicherheit (LF4)</t>
+  </si>
+  <si>
+    <t>UML-Anwendungsfalldiagramme erstellen</t>
+  </si>
+  <si>
+    <t>Struktogramme erstellen</t>
+  </si>
+  <si>
+    <t>Struktogramme mithilfe des Schreibtischtest prüfen</t>
+  </si>
+  <si>
+    <t>Netzwerkkomponenten unterscheiden</t>
+  </si>
+  <si>
+    <t>Verkabelung von Netzwerkkomponenten dimensionieren</t>
+  </si>
+  <si>
+    <t>IPv4-Netzwerke planen</t>
+  </si>
+  <si>
+    <t>Cybersecurity Grundlagen (LinkedIn Learning)</t>
+  </si>
+  <si>
+    <t>Datenbanken abfragen (bis Kap. 14 inkl.)</t>
   </si>
 </sst>
 </file>
@@ -272,11 +293,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -290,11 +309,38 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -752,245 +798,293 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DB9513-9E88-4020-9A13-204A732F2DD8}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.21875" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" customWidth="1"/>
-    <col min="4" max="4" width="47.21875" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="2.88671875" customWidth="1"/>
-    <col min="7" max="7" width="47.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="55.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="7"/>
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="G3" s="8" t="s">
+      <c r="E3" s="7"/>
+      <c r="G3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="E4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="E5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="E6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="E7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="H7" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="E8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="E9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H9" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="E10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="3" t="s">
+      <c r="H10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="E11" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="D14" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="G14" s="8" t="s">
+      <c r="B14" s="7"/>
+      <c r="D14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="G14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="B17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1004,16 +1098,34 @@
     <mergeCell ref="D14:E14"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:B8">
-    <cfRule type="cellIs" dxfId="20" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="76" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="77" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="78" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="iconSet" priority="58">
+    <cfRule type="iconSet" priority="79">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:B17">
+    <cfRule type="cellIs" dxfId="20" priority="80" operator="equal">
+      <formula>"in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="81" operator="equal">
+      <formula>"Offen"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="82" operator="equal">
+      <formula>"Erledigt"</formula>
+    </cfRule>
+    <cfRule type="iconSet" priority="83">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1022,27 +1134,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="iconSet" priority="38">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E11">
-    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
+    <cfRule type="iconSet" priority="59">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E11 H15:H20">
+    <cfRule type="cellIs" dxfId="17" priority="48" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="49" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="50" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E10">
-    <cfRule type="iconSet" priority="46">
+    <cfRule type="iconSet" priority="67">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1051,6 +1163,62 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
+    <cfRule type="iconSet" priority="51">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="iconSet" priority="55">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H10">
+    <cfRule type="cellIs" dxfId="14" priority="44" operator="equal">
+      <formula>"in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="45" operator="equal">
+      <formula>"Offen"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="46" operator="equal">
+      <formula>"Erledigt"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H9">
+    <cfRule type="iconSet" priority="63">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="iconSet" priority="47">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:H16">
+    <cfRule type="iconSet" priority="25">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
     <cfRule type="iconSet" priority="30">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1059,101 +1227,90 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="iconSet" priority="34">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H10">
-    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
+  <conditionalFormatting sqref="H20">
+    <cfRule type="iconSet" priority="29">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="iconSet" priority="21">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="iconSet" priority="20">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B20">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H9">
-    <cfRule type="iconSet" priority="42">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="iconSet" priority="26">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B18">
-    <cfRule type="cellIs" dxfId="11" priority="59" operator="equal">
+  <conditionalFormatting sqref="B20">
+    <cfRule type="iconSet" priority="16">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B20">
+    <cfRule type="iconSet" priority="14">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="iconSet" priority="13">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
-    <cfRule type="iconSet" priority="62">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16:H17">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"in Bearbeitung"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"Offen"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
-      <formula>"Erledigt"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
-    <cfRule type="iconSet" priority="9">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="iconSet" priority="8">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
-    <cfRule type="iconSet" priority="4">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+    <cfRule type="iconSet" priority="12">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
@@ -1164,8 +1321,17 @@
       <formula>"Erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="iconSet" priority="4">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C8 E4:F11 H4:H10 B15:B18 H15:H17" xr:uid="{EC34E9F4-7F72-4106-BC88-1EE30967E81D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C8 E4:F11 H4:H10 B15:B21 H15:H20 E15" xr:uid="{EC34E9F4-7F72-4106-BC88-1EE30967E81D}">
       <formula1>"Offen, in Bearbeitung, Erledigt"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Lernstand um IT-Sicherheit aktualisiert
</commit_message>
<xml_diff>
--- a/docs/material/Lernstand.xlsx
+++ b/docs/material/Lernstand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\GitHub\MMBbS_KIT_PVAP1\docs\material\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://multimediabbshannover-my.sharepoint.com/personal/neumann_mmbbs_de/Documents/Desktop/GitHub/MMBbS_KIT_PVAP1/docs/material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E72F58-C897-479D-9249-1A9947046433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{C7E72F58-C897-479D-9249-1A9947046433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AE13F5C-D114-4058-AEE5-D142695A1B34}"/>
   <bookViews>
-    <workbookView xWindow="17970" yWindow="16035" windowWidth="20295" windowHeight="15525" xr2:uid="{B7884D5C-17C3-4F72-B534-6B15B5BBA262}"/>
+    <workbookView xWindow="19200" yWindow="15960" windowWidth="32400" windowHeight="15585" xr2:uid="{B7884D5C-17C3-4F72-B534-6B15B5BBA262}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>Projektmanagement (div. LF)</t>
   </si>
@@ -161,10 +161,28 @@
     <t>IPv4-Netzwerke planen</t>
   </si>
   <si>
-    <t>Cybersecurity Grundlagen (LinkedIn Learning)</t>
-  </si>
-  <si>
     <t>Datenbanken abfragen (bis Kap. 14 inkl.)</t>
+  </si>
+  <si>
+    <t>Grundlagen der Informationssicherheit anwenden</t>
+  </si>
+  <si>
+    <t>IT-Grundschutz planen</t>
+  </si>
+  <si>
+    <t>DSGVO-konform handeln</t>
+  </si>
+  <si>
+    <t>Abwehr von Angriffen planen</t>
+  </si>
+  <si>
+    <t>Verfügbarkeit sicherstellen</t>
+  </si>
+  <si>
+    <t>Integrität gewährleisten</t>
+  </si>
+  <si>
+    <t>Vertraulichkeit herstellen</t>
   </si>
 </sst>
 </file>
@@ -303,23 +321,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="21">
     <dxf>
       <font>
         <b/>
@@ -366,6 +384,13 @@
       <font>
         <b/>
         <i val="0"/>
+        <color theme="7" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color rgb="FF00B050"/>
       </font>
     </dxf>
@@ -380,6 +405,20 @@
       <font>
         <b/>
         <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color theme="7" tint="0.39994506668294322"/>
       </font>
     </dxf>
@@ -387,6 +426,20 @@
       <font>
         <b/>
         <i val="0"/>
+        <color theme="7" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color rgb="FF00B050"/>
       </font>
     </dxf>
@@ -394,6 +447,13 @@
       <font>
         <b/>
         <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color rgb="FFC00000"/>
       </font>
     </dxf>
@@ -415,77 +475,14 @@
       <font>
         <b/>
         <i val="0"/>
+        <color theme="7" tint="0.39994506668294322"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="7" tint="0.39994506668294322"/>
       </font>
     </dxf>
   </dxfs>
@@ -502,9 +499,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -542,7 +539,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -648,7 +645,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -790,7 +787,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -800,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DB9513-9E88-4020-9A13-204A732F2DD8}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,36 +823,36 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="9"/>
+      <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="G3" s="6" t="s">
+      <c r="E3" s="9"/>
+      <c r="G3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -863,19 +860,19 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -883,19 +880,19 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -903,19 +900,19 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -923,19 +920,19 @@
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -943,13 +940,13 @@
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -957,13 +954,13 @@
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -971,42 +968,42 @@
       <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="D14" s="6" t="s">
+      <c r="B14" s="9"/>
+      <c r="D14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="G14" s="6" t="s">
+      <c r="E14" s="9"/>
+      <c r="G14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="B15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1014,13 +1011,19 @@
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1028,13 +1031,19 @@
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1042,13 +1051,19 @@
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1056,13 +1071,19 @@
       <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1070,13 +1091,19 @@
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1084,7 +1111,13 @@
       <c r="A21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1098,15 +1131,138 @@
     <mergeCell ref="D14:E14"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:B8">
-    <cfRule type="cellIs" dxfId="23" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="93" operator="equal">
+      <formula>"Offen"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="92" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="94" operator="equal">
+      <formula>"Erledigt"</formula>
+    </cfRule>
+    <cfRule type="iconSet" priority="95">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:B17">
+    <cfRule type="iconSet" priority="99">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:B21">
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
+      <formula>"in Bearbeitung"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
       <formula>"Offen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
       <formula>"Erledigt"</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B20">
+    <cfRule type="iconSet" priority="30">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="iconSet" priority="29">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="iconSet" priority="32">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="iconSet" priority="28">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="iconSet" priority="75">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E11 H15:H20">
+    <cfRule type="cellIs" dxfId="14" priority="66" operator="equal">
+      <formula>"Erledigt"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="65" operator="equal">
+      <formula>"Offen"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="64" operator="equal">
+      <formula>"in Bearbeitung"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E10">
+    <cfRule type="iconSet" priority="83">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="iconSet" priority="67">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="iconSet" priority="71">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H10">
+    <cfRule type="cellIs" dxfId="8" priority="61" operator="equal">
+      <formula>"Offen"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="62" operator="equal">
+      <formula>"Erledigt"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="60" operator="equal">
+      <formula>"in Bearbeitung"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H9">
     <cfRule type="iconSet" priority="79">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1115,83 +1271,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:B17">
-    <cfRule type="cellIs" dxfId="20" priority="80" operator="equal">
-      <formula>"in Bearbeitung"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="81" operator="equal">
-      <formula>"Offen"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="82" operator="equal">
-      <formula>"Erledigt"</formula>
-    </cfRule>
-    <cfRule type="iconSet" priority="83">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="iconSet" priority="59">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E11 H15:H20">
-    <cfRule type="cellIs" dxfId="17" priority="48" operator="equal">
-      <formula>"in Bearbeitung"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="49" operator="equal">
-      <formula>"Offen"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="50" operator="equal">
-      <formula>"Erledigt"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E10">
-    <cfRule type="iconSet" priority="67">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="iconSet" priority="51">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="iconSet" priority="55">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H10">
-    <cfRule type="cellIs" dxfId="14" priority="44" operator="equal">
-      <formula>"in Bearbeitung"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="45" operator="equal">
-      <formula>"Offen"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="46" operator="equal">
-      <formula>"Erledigt"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H9">
+  <conditionalFormatting sqref="H10">
     <cfRule type="iconSet" priority="63">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1200,17 +1280,26 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="iconSet" priority="47">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H15:H16">
-    <cfRule type="iconSet" priority="25">
+    <cfRule type="iconSet" priority="41">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="iconSet" priority="37">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="iconSet" priority="36">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1219,7 +1308,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="iconSet" priority="30">
+    <cfRule type="iconSet" priority="46">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1228,89 +1317,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="iconSet" priority="29">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="iconSet" priority="21">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
-    <cfRule type="iconSet" priority="20">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:B20">
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
-      <formula>"in Bearbeitung"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
-      <formula>"Offen"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
-      <formula>"Erledigt"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="iconSet" priority="16">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:B20">
-    <cfRule type="iconSet" priority="14">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="iconSet" priority="13">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
-      <formula>"in Bearbeitung"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
-      <formula>"Offen"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
-      <formula>"Erledigt"</formula>
-    </cfRule>
-    <cfRule type="iconSet" priority="12">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
+    <cfRule type="iconSet" priority="45">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:E17">
+    <cfRule type="iconSet" priority="8">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:E21">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"in Bearbeitung"</formula>
     </cfRule>
@@ -1321,7 +1345,34 @@
       <formula>"Erledigt"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
+  <conditionalFormatting sqref="E18:E20">
+    <cfRule type="iconSet" priority="6">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="iconSet" priority="5">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="iconSet" priority="7">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
     <cfRule type="iconSet" priority="4">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
@@ -1331,7 +1382,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C8 E4:F11 H4:H10 B15:B21 H15:H20 E15" xr:uid="{EC34E9F4-7F72-4106-BC88-1EE30967E81D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C8 E4:F11 H4:H10 B15:B21 H15:H20 E15:E21" xr:uid="{EC34E9F4-7F72-4106-BC88-1EE30967E81D}">
       <formula1>"Offen, in Bearbeitung, Erledigt"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>